<commit_message>
Modified some files in ranger2
</commit_message>
<xml_diff>
--- a/xpmsrequests/data/ExcelData/TestSuiteData.xlsx
+++ b/xpmsrequests/data/ExcelData/TestSuiteData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">TCID</t>
   </si>
@@ -31,12 +31,6 @@
     <t xml:space="preserve">FileName</t>
   </si>
   <si>
-    <t xml:space="preserve">Col2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col3</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC01</t>
   </si>
   <si>
@@ -46,25 +40,7 @@
     <t xml:space="preserve">CMS1500_1.png</t>
   </si>
   <si>
-    <t xml:space="preserve">tc01col2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tc01col3</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TempTC02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tc02col1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tc02col2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tc02col3</t>
   </si>
 </sst>
 </file>
@@ -74,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -95,6 +71,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,8 +120,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,18 +146,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,45 +168,24 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>